<commit_message>
Accommodate max and min required proportions
</commit_message>
<xml_diff>
--- a/TerrestrialAIM_DataAnalysis_Template.xlsx
+++ b/TerrestrialAIM_DataAnalysis_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="-285" windowWidth="24240" windowHeight="8175" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="1365" yWindow="-285" windowWidth="24240" windowHeight="8175" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4100" uniqueCount="1364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4109" uniqueCount="1366">
   <si>
     <t>Management Question</t>
   </si>
@@ -3946,9 +3946,6 @@
     <t>Acceptable</t>
   </si>
   <si>
-    <t>Minimum Proportion</t>
-  </si>
-  <si>
     <t>Benchmark Source</t>
   </si>
   <si>
@@ -4352,6 +4349,15 @@
   </si>
   <si>
     <t>Sagebrush Cover  (%, first hit)</t>
+  </si>
+  <si>
+    <t>Required Proportion</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Proportion Relation</t>
   </si>
 </sst>
 </file>
@@ -4543,7 +4549,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -5076,11 +5082,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5415,6 +5471,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6788,13 +6856,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -6851,13 +6919,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
@@ -6914,13 +6982,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -6932,8 +7000,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="14716125" y="0"/>
-          <a:ext cx="2162175" cy="428625"/>
+          <a:off x="15525750" y="0"/>
+          <a:ext cx="2162175" cy="371475"/>
           <a:chOff x="12353925" y="3705226"/>
           <a:chExt cx="2162175" cy="371474"/>
         </a:xfrm>
@@ -7051,13 +7119,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
@@ -7113,13 +7181,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -8474,8 +8542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8489,23 +8557,22 @@
     <col min="7" max="7" width="7.42578125" style="4" customWidth="1"/>
     <col min="8" max="8" width="6.7109375" style="4" customWidth="1"/>
     <col min="9" max="9" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="3"/>
-    <col min="15" max="15" width="8" style="3" customWidth="1"/>
-    <col min="16" max="16" width="33.85546875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.140625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="3"/>
+    <col min="16" max="16" width="8" style="3" customWidth="1"/>
+    <col min="17" max="17" width="33.85546875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" customWidth="1"/>
     <col min="19" max="19" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="28" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="28" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="94" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="C1" s="98" t="s">
         <v>1219</v>
@@ -8531,20 +8598,20 @@
       <c r="J1" s="102" t="s">
         <v>1220</v>
       </c>
-      <c r="K1" s="95" t="s">
-        <v>1228</v>
-      </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="30"/>
+      <c r="K1" s="102" t="s">
+        <v>1365</v>
+      </c>
+      <c r="L1" s="95" t="s">
+        <v>1363</v>
+      </c>
+      <c r="M1" s="29"/>
       <c r="N1" s="30"/>
       <c r="O1" s="30"/>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="30"/>
+      <c r="Q1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="7" t="s">
-        <v>889</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="R1" s="7" t="s">
         <v>889</v>
       </c>
     </row>
@@ -8562,7 +8629,7 @@
         <v>60</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="F2" s="54" t="s">
         <v>17</v>
@@ -8579,18 +8646,18 @@
       <c r="J2" s="103" t="s">
         <v>1223</v>
       </c>
-      <c r="K2" s="58">
+      <c r="K2" s="117" t="s">
+        <v>891</v>
+      </c>
+      <c r="L2" s="58">
         <v>0.7</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="6"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="6"/>
+      <c r="Q2" s="23" t="s">
         <v>14</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>892</v>
       </c>
       <c r="R2" t="s">
         <v>892</v>
@@ -8616,7 +8683,7 @@
         <v>892</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="G3" s="40" t="s">
         <v>892</v>
@@ -8630,8 +8697,13 @@
       <c r="J3" s="104" t="s">
         <v>1224</v>
       </c>
-      <c r="K3" s="42"/>
-      <c r="P3" s="23" t="s">
+      <c r="K3" s="118" t="s">
+        <v>889</v>
+      </c>
+      <c r="L3" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="Q3" s="23" t="s">
         <v>15</v>
       </c>
       <c r="S3" t="s">
@@ -8655,7 +8727,7 @@
         <v>889</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="G4" s="40" t="s">
         <v>892</v>
@@ -8669,11 +8741,12 @@
       <c r="J4" s="104" t="s">
         <v>1225</v>
       </c>
-      <c r="K4" s="42"/>
-      <c r="P4" s="23" t="s">
+      <c r="K4" s="118"/>
+      <c r="L4" s="42"/>
+      <c r="Q4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>890</v>
       </c>
       <c r="S4" t="s">
@@ -8697,7 +8770,7 @@
         <v>889</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="G5" s="40" t="s">
         <v>892</v>
@@ -8711,11 +8784,17 @@
       <c r="J5" s="104" t="s">
         <v>1223</v>
       </c>
-      <c r="K5" s="42">
+      <c r="K5" s="118" t="s">
+        <v>891</v>
+      </c>
+      <c r="L5" s="42">
         <v>0.7</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="Q5" s="23" t="s">
         <v>11</v>
+      </c>
+      <c r="R5" t="s">
+        <v>891</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -8735,7 +8814,7 @@
         <v>892</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>889</v>
@@ -8749,9 +8828,17 @@
       <c r="J6" s="105" t="s">
         <v>1226</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="P6" s="23" t="s">
+      <c r="K6" s="119" t="s">
+        <v>889</v>
+      </c>
+      <c r="L6" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="Q6" s="23" t="s">
         <v>12</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1364</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -8771,7 +8858,7 @@
         <v>892</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>892</v>
@@ -8785,10 +8872,13 @@
       <c r="J7" s="105" t="s">
         <v>1227</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="119" t="s">
+        <v>891</v>
+      </c>
+      <c r="L7" s="15">
         <v>0.9</v>
       </c>
-      <c r="P7" s="23" t="s">
+      <c r="Q7" s="23" t="s">
         <v>40</v>
       </c>
     </row>
@@ -8809,7 +8899,7 @@
         <v>889</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>892</v>
@@ -8823,8 +8913,13 @@
       <c r="J8" s="105" t="s">
         <v>1226</v>
       </c>
-      <c r="K8" s="15"/>
-      <c r="P8" s="23" t="s">
+      <c r="K8" s="119" t="s">
+        <v>889</v>
+      </c>
+      <c r="L8" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="Q8" s="23" t="s">
         <v>29</v>
       </c>
     </row>
@@ -8845,7 +8940,7 @@
         <v>889</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>889</v>
@@ -8859,10 +8954,13 @@
       <c r="J9" s="105" t="s">
         <v>1227</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="119" t="s">
+        <v>1364</v>
+      </c>
+      <c r="L9" s="15">
         <v>0.75</v>
       </c>
-      <c r="P9" s="23" t="s">
+      <c r="Q9" s="23" t="s">
         <v>32</v>
       </c>
     </row>
@@ -8883,7 +8981,7 @@
         <v>892</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>889</v>
@@ -8897,8 +8995,13 @@
       <c r="J10" s="105" t="s">
         <v>1226</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="P10" s="23" t="s">
+      <c r="K10" s="119" t="s">
+        <v>892</v>
+      </c>
+      <c r="L10" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="Q10" s="23" t="s">
         <v>31</v>
       </c>
     </row>
@@ -8913,8 +9016,9 @@
       <c r="H11" s="11"/>
       <c r="I11" s="13"/>
       <c r="J11" s="105"/>
-      <c r="K11" s="15"/>
-      <c r="P11" s="23" t="s">
+      <c r="K11" s="119"/>
+      <c r="L11" s="15"/>
+      <c r="Q11" s="23" t="s">
         <v>28</v>
       </c>
     </row>
@@ -8929,8 +9033,9 @@
       <c r="H12" s="11"/>
       <c r="I12" s="13"/>
       <c r="J12" s="105"/>
-      <c r="K12" s="15"/>
-      <c r="P12" s="23" t="s">
+      <c r="K12" s="119"/>
+      <c r="L12" s="15"/>
+      <c r="Q12" s="23" t="s">
         <v>33</v>
       </c>
     </row>
@@ -8945,8 +9050,9 @@
       <c r="H13" s="11"/>
       <c r="I13" s="13"/>
       <c r="J13" s="105"/>
-      <c r="K13" s="15"/>
-      <c r="P13" s="23" t="s">
+      <c r="K13" s="119"/>
+      <c r="L13" s="15"/>
+      <c r="Q13" s="23" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8961,8 +9067,9 @@
       <c r="H14" s="11"/>
       <c r="I14" s="13"/>
       <c r="J14" s="105"/>
-      <c r="K14" s="15"/>
-      <c r="P14" s="23" t="s">
+      <c r="K14" s="119"/>
+      <c r="L14" s="15"/>
+      <c r="Q14" s="23" t="s">
         <v>44</v>
       </c>
     </row>
@@ -8977,8 +9084,9 @@
       <c r="H15" s="11"/>
       <c r="I15" s="13"/>
       <c r="J15" s="105"/>
-      <c r="K15" s="15"/>
-      <c r="P15" s="23" t="s">
+      <c r="K15" s="119"/>
+      <c r="L15" s="15"/>
+      <c r="Q15" s="23" t="s">
         <v>45</v>
       </c>
     </row>
@@ -8993,12 +9101,13 @@
       <c r="H16" s="11"/>
       <c r="I16" s="13"/>
       <c r="J16" s="105"/>
-      <c r="K16" s="15"/>
-      <c r="P16" s="23" t="s">
+      <c r="K16" s="119"/>
+      <c r="L16" s="15"/>
+      <c r="Q16" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="96"/>
@@ -9009,12 +9118,13 @@
       <c r="H17" s="11"/>
       <c r="I17" s="13"/>
       <c r="J17" s="105"/>
-      <c r="K17" s="15"/>
-      <c r="P17" s="23" t="s">
+      <c r="K17" s="119"/>
+      <c r="L17" s="15"/>
+      <c r="Q17" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="96"/>
@@ -9025,12 +9135,13 @@
       <c r="H18" s="11"/>
       <c r="I18" s="13"/>
       <c r="J18" s="105"/>
-      <c r="K18" s="15"/>
-      <c r="P18" s="23" t="s">
+      <c r="K18" s="119"/>
+      <c r="L18" s="15"/>
+      <c r="Q18" s="23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="96"/>
@@ -9041,12 +9152,13 @@
       <c r="H19" s="11"/>
       <c r="I19" s="13"/>
       <c r="J19" s="105"/>
-      <c r="K19" s="15"/>
-      <c r="P19" s="23" t="s">
+      <c r="K19" s="119"/>
+      <c r="L19" s="15"/>
+      <c r="Q19" s="23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="96"/>
@@ -9057,12 +9169,13 @@
       <c r="H20" s="11"/>
       <c r="I20" s="13"/>
       <c r="J20" s="105"/>
-      <c r="K20" s="15"/>
-      <c r="P20" s="23" t="s">
+      <c r="K20" s="119"/>
+      <c r="L20" s="15"/>
+      <c r="Q20" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
       <c r="C21" s="96"/>
@@ -9073,12 +9186,13 @@
       <c r="H21" s="11"/>
       <c r="I21" s="13"/>
       <c r="J21" s="105"/>
-      <c r="K21" s="15"/>
-      <c r="P21" s="23" t="s">
+      <c r="K21" s="119"/>
+      <c r="L21" s="15"/>
+      <c r="Q21" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="96"/>
@@ -9089,12 +9203,13 @@
       <c r="H22" s="11"/>
       <c r="I22" s="13"/>
       <c r="J22" s="105"/>
-      <c r="K22" s="15"/>
-      <c r="P22" s="23" t="s">
+      <c r="K22" s="119"/>
+      <c r="L22" s="15"/>
+      <c r="Q22" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="96"/>
@@ -9105,12 +9220,13 @@
       <c r="H23" s="11"/>
       <c r="I23" s="13"/>
       <c r="J23" s="105"/>
-      <c r="K23" s="15"/>
-      <c r="P23" s="23" t="s">
+      <c r="K23" s="119"/>
+      <c r="L23" s="15"/>
+      <c r="Q23" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="96"/>
@@ -9121,12 +9237,13 @@
       <c r="H24" s="11"/>
       <c r="I24" s="13"/>
       <c r="J24" s="105"/>
-      <c r="K24" s="15"/>
-      <c r="P24" s="23" t="s">
+      <c r="K24" s="119"/>
+      <c r="L24" s="15"/>
+      <c r="Q24" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="96"/>
@@ -9137,12 +9254,13 @@
       <c r="H25" s="11"/>
       <c r="I25" s="13"/>
       <c r="J25" s="105"/>
-      <c r="K25" s="15"/>
-      <c r="P25" s="23" t="s">
+      <c r="K25" s="119"/>
+      <c r="L25" s="15"/>
+      <c r="Q25" s="23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="96"/>
@@ -9153,12 +9271,13 @@
       <c r="H26" s="11"/>
       <c r="I26" s="13"/>
       <c r="J26" s="105"/>
-      <c r="K26" s="15"/>
-      <c r="P26" s="23" t="s">
+      <c r="K26" s="119"/>
+      <c r="L26" s="15"/>
+      <c r="Q26" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="20"/>
       <c r="C27" s="97"/>
@@ -9169,98 +9288,99 @@
       <c r="H27" s="12"/>
       <c r="I27" s="14"/>
       <c r="J27" s="106"/>
-      <c r="K27" s="16"/>
-      <c r="P27" s="23" t="s">
+      <c r="K27" s="120"/>
+      <c r="L27" s="16"/>
+      <c r="Q27" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D28" s="10"/>
       <c r="E28" s="8"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
-      <c r="K28" s="9"/>
-      <c r="P28" s="23" t="s">
+      <c r="L28" s="9"/>
+      <c r="Q28" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P29" s="23" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q29" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P30" s="23" t="s">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q30" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P31" s="23" t="s">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q31" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P32" s="23" t="s">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q32" s="23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P33" s="23" t="s">
+    <row r="33" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q33" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P34" s="23" t="s">
+    <row r="34" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q34" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P35" s="23" t="s">
+    <row r="35" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q35" s="23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P36" s="23" t="s">
+    <row r="36" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q36" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P37" s="23" t="s">
+    <row r="37" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q37" s="23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P38" s="23" t="s">
+    <row r="38" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q38" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P39" s="23" t="s">
+    <row r="39" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q39" s="23" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="P2:P40">
-    <sortCondition ref="P3"/>
+  <sortState ref="Q2:Q40">
+    <sortCondition ref="Q3"/>
   </sortState>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
-      <formula1>$P$1:$P$39</formula1>
+      <formula1>$Q$1:$Q$39</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28">
-      <formula1>$Q$1:$Q$6</formula1>
+      <formula1>$R$1:$R$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28">
-      <formula1>$P$1:$P$37</formula1>
+      <formula1>$Q$1:$Q$37</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I28">
       <formula1>$S$2:$S$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E27">
-      <formula1>$Q$1:$Q$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E27 E2 G2:G27">
+      <formula1>$R$1:$R$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G27">
-      <formula1>$R$1:$R$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K27">
+      <formula1>$R$1:$R$7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9379,121 +9499,121 @@
         <v>10</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="P1" s="34" t="s">
+        <v>1294</v>
+      </c>
+      <c r="Q1" s="34" t="s">
         <v>1295</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="R1" s="34" t="s">
         <v>1296</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="S1" s="34" t="s">
+        <v>1298</v>
+      </c>
+      <c r="T1" s="34" t="s">
+        <v>1299</v>
+      </c>
+      <c r="U1" s="34" t="s">
+        <v>1300</v>
+      </c>
+      <c r="V1" s="34" t="s">
+        <v>1301</v>
+      </c>
+      <c r="W1" s="34" t="s">
+        <v>1302</v>
+      </c>
+      <c r="X1" s="34" t="s">
+        <v>1303</v>
+      </c>
+      <c r="Y1" s="34" t="s">
+        <v>1304</v>
+      </c>
+      <c r="Z1" s="34" t="s">
+        <v>1305</v>
+      </c>
+      <c r="AA1" s="34" t="s">
+        <v>1306</v>
+      </c>
+      <c r="AB1" s="34" t="s">
+        <v>1307</v>
+      </c>
+      <c r="AC1" s="34" t="s">
+        <v>1308</v>
+      </c>
+      <c r="AD1" s="34" t="s">
+        <v>1309</v>
+      </c>
+      <c r="AE1" s="34" t="s">
+        <v>1310</v>
+      </c>
+      <c r="AF1" s="34" t="s">
+        <v>1311</v>
+      </c>
+      <c r="AG1" s="34" t="s">
+        <v>1312</v>
+      </c>
+      <c r="AH1" s="34" t="s">
+        <v>1313</v>
+      </c>
+      <c r="AI1" s="34" t="s">
+        <v>1314</v>
+      </c>
+      <c r="AJ1" s="34" t="s">
+        <v>1315</v>
+      </c>
+      <c r="AK1" s="34" t="s">
+        <v>1316</v>
+      </c>
+      <c r="AL1" s="34" t="s">
         <v>1297</v>
       </c>
-      <c r="S1" s="34" t="s">
-        <v>1299</v>
-      </c>
-      <c r="T1" s="34" t="s">
-        <v>1300</v>
-      </c>
-      <c r="U1" s="34" t="s">
-        <v>1301</v>
-      </c>
-      <c r="V1" s="34" t="s">
-        <v>1302</v>
-      </c>
-      <c r="W1" s="34" t="s">
-        <v>1303</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>1304</v>
-      </c>
-      <c r="Y1" s="34" t="s">
-        <v>1305</v>
-      </c>
-      <c r="Z1" s="34" t="s">
-        <v>1306</v>
-      </c>
-      <c r="AA1" s="34" t="s">
-        <v>1307</v>
-      </c>
-      <c r="AB1" s="34" t="s">
-        <v>1308</v>
-      </c>
-      <c r="AC1" s="34" t="s">
-        <v>1309</v>
-      </c>
-      <c r="AD1" s="34" t="s">
-        <v>1310</v>
-      </c>
-      <c r="AE1" s="34" t="s">
-        <v>1311</v>
-      </c>
-      <c r="AF1" s="34" t="s">
-        <v>1312</v>
-      </c>
-      <c r="AG1" s="34" t="s">
-        <v>1313</v>
-      </c>
-      <c r="AH1" s="34" t="s">
-        <v>1314</v>
-      </c>
-      <c r="AI1" s="34" t="s">
-        <v>1315</v>
-      </c>
-      <c r="AJ1" s="34" t="s">
-        <v>1316</v>
-      </c>
-      <c r="AK1" s="34" t="s">
+      <c r="AM1" s="34" t="s">
+        <v>1264</v>
+      </c>
+      <c r="AN1" s="34" t="s">
+        <v>1266</v>
+      </c>
+      <c r="AO1" s="34" t="s">
+        <v>1268</v>
+      </c>
+      <c r="AP1" s="34" t="s">
+        <v>1270</v>
+      </c>
+      <c r="AQ1" s="34" t="s">
+        <v>1272</v>
+      </c>
+      <c r="AR1" s="34" t="s">
+        <v>1274</v>
+      </c>
+      <c r="AS1" s="34" t="s">
         <v>1317</v>
       </c>
-      <c r="AL1" s="34" t="s">
-        <v>1298</v>
-      </c>
-      <c r="AM1" s="34" t="s">
-        <v>1265</v>
-      </c>
-      <c r="AN1" s="34" t="s">
-        <v>1267</v>
-      </c>
-      <c r="AO1" s="34" t="s">
-        <v>1269</v>
-      </c>
-      <c r="AP1" s="34" t="s">
-        <v>1271</v>
-      </c>
-      <c r="AQ1" s="34" t="s">
-        <v>1273</v>
-      </c>
-      <c r="AR1" s="34" t="s">
-        <v>1275</v>
-      </c>
-      <c r="AS1" s="34" t="s">
-        <v>1318</v>
-      </c>
       <c r="AT1" s="34" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AU1" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="AV1" s="34" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="AW1" s="34" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="AX1" s="34" t="s">
         <v>50</v>
@@ -82988,8 +83108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -83004,725 +83124,725 @@
         <v>898</v>
       </c>
       <c r="B1" s="34" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>1293</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C2" t="s">
         <v>1230</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1295</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1231</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B3" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C3" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B4" t="s">
         <v>1233</v>
       </c>
-      <c r="B4" t="s">
-        <v>1234</v>
-      </c>
       <c r="C4" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B5" t="s">
         <v>1235</v>
       </c>
-      <c r="B5" t="s">
-        <v>1236</v>
-      </c>
       <c r="C5" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B6" t="s">
         <v>1237</v>
       </c>
-      <c r="B6" t="s">
-        <v>1238</v>
-      </c>
       <c r="C6" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B7" t="s">
         <v>1239</v>
       </c>
-      <c r="B7" t="s">
-        <v>1240</v>
-      </c>
       <c r="C7" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B8" t="s">
         <v>1241</v>
       </c>
-      <c r="B8" t="s">
-        <v>1242</v>
-      </c>
       <c r="C8" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B9" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C9" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B10" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="C10" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B11" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C11" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B12" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="C12" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B13" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="C13" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B14" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="C14" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B15" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="C15" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B16" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C16" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B17" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="C17" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B18" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C18" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B19" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C19" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B20" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="C20" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B21" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C21" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B22" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C22" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B23" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="C23" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B24" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="C24" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B25" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C25" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B26" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="C26" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B27" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="C27" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B28" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="C28" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B29" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="C29" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B30" t="s">
         <v>1264</v>
       </c>
-      <c r="B30" t="s">
-        <v>1265</v>
-      </c>
       <c r="C30" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B31" t="s">
         <v>1266</v>
       </c>
-      <c r="B31" t="s">
-        <v>1267</v>
-      </c>
       <c r="C31" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B32" t="s">
         <v>1268</v>
       </c>
-      <c r="B32" t="s">
-        <v>1269</v>
-      </c>
       <c r="C32" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B33" t="s">
         <v>1270</v>
       </c>
-      <c r="B33" t="s">
-        <v>1271</v>
-      </c>
       <c r="C33" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B34" t="s">
         <v>1272</v>
       </c>
-      <c r="B34" t="s">
-        <v>1273</v>
-      </c>
       <c r="C34" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B35" t="s">
         <v>1274</v>
       </c>
-      <c r="B35" t="s">
-        <v>1275</v>
-      </c>
       <c r="C35" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B36" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C36" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B37" t="s">
         <v>1277</v>
       </c>
-      <c r="B37" t="s">
-        <v>1278</v>
-      </c>
       <c r="C37" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B38" t="s">
         <v>1279</v>
       </c>
-      <c r="B38" t="s">
-        <v>1280</v>
-      </c>
       <c r="C38" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B39" t="s">
         <v>1281</v>
       </c>
-      <c r="B39" t="s">
-        <v>1282</v>
-      </c>
       <c r="C39" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B40" t="s">
         <v>1283</v>
       </c>
-      <c r="B40" t="s">
-        <v>1284</v>
-      </c>
       <c r="C40" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C41" t="s">
         <v>1285</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1319</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1286</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B42" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C42" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B43" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="C43" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B44" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="C44" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B45" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="C45" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B46" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="C46" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="B47" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="C47" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B48" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="C48" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B49" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C49" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B50" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="C50" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="B51" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="C51" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B52" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C52" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B53" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="C53" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B54" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="C54" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B55" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="C55" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="B56" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C56" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B57" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C57" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B58" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C58" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B59" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="C59" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B60" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="C60" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B61" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C61" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B62" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="C62" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B63" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="C63" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B64" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="C64" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B65" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="C65" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B66" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="C66" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>